<commit_message>
Cleaned up output formatting for files - now uses a vertical table
</commit_message>
<xml_diff>
--- a/test_data/Glop_Pot/sketchsheets/CATALOG_sketchsheets.xlsx
+++ b/test_data/Glop_Pot/sketchsheets/CATALOG_sketchsheets.xlsx
@@ -1,94 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/124411/Dropbox/calcyte.js/test_data/Glop_Pot/sketchsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="620" windowWidth="28560" windowHeight="17380" tabRatio="500" activeTab="1"/>
-  </bookViews>
   <sheets>
     <sheet name="Collection" sheetId="1" r:id="rId1"/>
     <sheet name="Files" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Sketch Sheets</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Metadata file for Glop Pot sketch sheets</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>sketch</t>
-  </si>
-  <si>
-    <t>FILE:Filename</t>
-  </si>
-  <si>
-    <t>RELATION:Creator*</t>
-  </si>
-  <si>
-    <t>RELATION:License</t>
-  </si>
-  <si>
-    <t>CP7Glopsketch01.jpg</t>
-  </si>
-  <si>
-    <t>Downstream from sump 2 to sump 1</t>
-  </si>
-  <si>
-    <t>Phil Maynard, Andreas Klocker</t>
-  </si>
-  <si>
-    <t>CC-BY</t>
-  </si>
-  <si>
-    <t>CP7Glopsketch02.jpg</t>
-  </si>
-  <si>
-    <t>Downstream from sump 1 to ladder</t>
-  </si>
-  <si>
-    <t>CP7Glopsketch03.jpg</t>
-  </si>
-  <si>
-    <t>In from tag to ladder</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,11 +51,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -454,121 +375,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Collection" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Collection"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Value</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Sketch Sheets</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Description</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Metadata file for Glop Pot sketch sheets</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B4" t="str">
+        <v>sketch</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Files" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Files"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>FILE:Filename</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>RELATION:Creator*</v>
+      </c>
+      <c r="D1" t="str">
+        <v>RELATION:License</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>CP7Glopsketch01.jpg</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Downstream from sump 2 to sump 1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Phil Maynard, Andreas Klocker</v>
+      </c>
+      <c r="D2" t="str">
+        <v>CC-BY</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>CP7Glopsketch02.jpg</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Downstream from sump 1 to ladder</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Phil Maynard, Andreas Klocker</v>
+      </c>
+      <c r="D3" t="str">
+        <v>CC-BY</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>CP7Glopsketch03.jpg</v>
+      </c>
+      <c r="B4" t="str">
+        <v>In from tag to ladder</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Phil Maynard, Andreas Klocker</v>
+      </c>
+      <c r="D4" t="str">
+        <v>CC-BY</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>